<commit_message>
V3 avec fichier de conf en paramètre
Ajout lancement avec fichier de conf, pour calibration avec Cayl ou avec PJ
</commit_message>
<xml_diff>
--- a/ajustements.xlsx
+++ b/ajustements.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\Qt_Dev\AGIV_Bench\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC1C786-6CEB-4090-8AA6-EDE393C6B150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="17835" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="1185" yWindow="1410" windowWidth="30675" windowHeight="19980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="1" r:id="rId1"/>
     <sheet name="Resistances" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>X0</t>
   </si>
@@ -85,13 +102,46 @@
   </si>
   <si>
     <t>R = Z + ((R-Rmin)/(Rmax-Rmin)) * G</t>
+  </si>
+  <si>
+    <t>réf X</t>
+  </si>
+  <si>
+    <t>réf Y</t>
+  </si>
+  <si>
+    <t>mes X</t>
+  </si>
+  <si>
+    <t>mes Y</t>
+  </si>
+  <si>
+    <t>Dréf</t>
+  </si>
+  <si>
+    <t>Dmes</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>pente mes</t>
+  </si>
+  <si>
+    <t>gain origine</t>
+  </si>
+  <si>
+    <t>gain corrigé</t>
+  </si>
+  <si>
+    <t>correction Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,13 +198,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -192,7 +250,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -226,6 +284,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -260,9 +319,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,21 +495,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:P19"/>
   <sheetViews>
     <sheetView topLeftCell="B3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C5" sqref="C5:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="2" customWidth="1"/>
     <col min="6" max="6" width="6.140625" customWidth="1"/>
     <col min="7" max="15" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>11</v>
       </c>
@@ -457,7 +517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:16">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -501,7 +561,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="3:16">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -515,7 +575,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="3:16">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>2</v>
       </c>
@@ -559,7 +619,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="8" spans="3:16">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>3</v>
       </c>
@@ -573,7 +633,7 @@
         <v>23.497800000000002</v>
       </c>
     </row>
-    <row r="9" spans="3:16">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>13</v>
       </c>
@@ -586,7 +646,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="10" spans="3:16">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -599,7 +659,7 @@
         <v>23.3978</v>
       </c>
     </row>
-    <row r="11" spans="3:16">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>4</v>
       </c>
@@ -616,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:16">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>5</v>
       </c>
@@ -633,7 +693,7 @@
         <v>0.99990598290598298</v>
       </c>
     </row>
-    <row r="13" spans="3:16">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>6</v>
       </c>
@@ -647,7 +707,7 @@
         <v>1.00023</v>
       </c>
     </row>
-    <row r="14" spans="3:16">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>7</v>
       </c>
@@ -664,7 +724,7 @@
         <v>1.0003240475600268</v>
       </c>
     </row>
-    <row r="15" spans="3:16" hidden="1">
+    <row r="15" spans="3:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>8</v>
       </c>
@@ -681,7 +741,7 @@
         <v>0.99967605741277821</v>
       </c>
     </row>
-    <row r="16" spans="3:16">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>9</v>
       </c>
@@ -695,7 +755,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>10</v>
       </c>
@@ -712,7 +772,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>15</v>
       </c>
@@ -726,19 +786,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B8:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
@@ -749,7 +809,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>2.0000000000000001E-4</v>
       </c>
@@ -757,7 +817,7 @@
         <v>1.004</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>0</v>
       </c>
@@ -769,7 +829,7 @@
         <v>2.105263157894737E-4</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>0.1</v>
       </c>
@@ -790,7 +850,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>-0.1</v>
       </c>
@@ -804,23 +864,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E13" s="3">
         <f>0.1/-475</f>
         <v>-2.105263157894737E-4</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H16">
         <v>476</v>
       </c>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20" s="3">
         <f>24/0.01</f>
         <v>2400</v>
@@ -832,13 +892,289 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A6:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>-0.43</v>
+      </c>
+      <c r="D7">
+        <v>-0.42</v>
+      </c>
+      <c r="E7">
+        <v>2.31E-3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>450</v>
+      </c>
+      <c r="D8" s="2">
+        <v>450</v>
+      </c>
+      <c r="E8" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="F8" s="4">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>448.34</v>
+      </c>
+      <c r="D9">
+        <v>448.53</v>
+      </c>
+      <c r="E9">
+        <v>23.485109999999999</v>
+      </c>
+      <c r="F9" s="3">
+        <v>23.497800000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <f>C8-C6</f>
+        <v>450</v>
+      </c>
+      <c r="D10">
+        <f>D8-D6</f>
+        <v>450</v>
+      </c>
+      <c r="F10">
+        <f>F8-F6</f>
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <f>C9-C7</f>
+        <v>448.77</v>
+      </c>
+      <c r="D11">
+        <f>D9-D7</f>
+        <v>448.95</v>
+      </c>
+      <c r="F11">
+        <f>F9-F7</f>
+        <v>23.3978</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <f>$C6-C7</f>
+        <v>0.43</v>
+      </c>
+      <c r="D12">
+        <f>$C6-D7</f>
+        <v>0.42</v>
+      </c>
+      <c r="E12">
+        <f>$D6-E7</f>
+        <v>-2.31E-3</v>
+      </c>
+      <c r="F12">
+        <f>$D6-F7</f>
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <f>C11/C10</f>
+        <v>0.99726666666666663</v>
+      </c>
+      <c r="D13">
+        <f>D11/D10</f>
+        <v>0.99766666666666659</v>
+      </c>
+      <c r="E13">
+        <f>(E9-E7)/($D8-$D6)</f>
+        <v>5.2183999999999994E-2</v>
+      </c>
+      <c r="F13">
+        <f>F11/F10</f>
+        <v>0.99990598290598298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1.0038750000000001</v>
+      </c>
+      <c r="F14">
+        <v>1.00023</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <f>C14/C13</f>
+        <v>1.002740824921452</v>
+      </c>
+      <c r="D15">
+        <f>D14/D13</f>
+        <v>1.0023387905111929</v>
+      </c>
+      <c r="E15">
+        <f>E14/E13</f>
+        <v>19.237218304461141</v>
+      </c>
+      <c r="F15">
+        <f>F14/F13</f>
+        <v>1.0003240475600268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="F17">
+        <v>9.7999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <f>C17-C12</f>
+        <v>-0.43</v>
+      </c>
+      <c r="E18">
+        <f>E17-E12</f>
+        <v>1.2109999999999999E-2</v>
+      </c>
+      <c r="F18">
+        <f>F17-F12</f>
+        <v>0.10980000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <f>C18*1/-486</f>
+        <v>8.847736625514403E-4</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f>C11*C15</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f>0.447979999999999/10000</f>
+        <v>4.4797999999999899E-5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>